<commit_message>
Updated Week 2 Homework
</commit_message>
<xml_diff>
--- a/AlexStrawn_Week2Homework.xlsx
+++ b/AlexStrawn_Week2Homework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theal\code\SavvyCoders\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC767164-CA1C-4162-87B0-FFC8E41608BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{65FD5B77-8947-47C9-8705-3920350D2B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId5"/>
+    <pivotCache cacheId="15" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="172">
   <si>
     <t>Expenses</t>
   </si>
@@ -549,6 +549,12 @@
   </si>
   <si>
     <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Years (Payment Date)</t>
+  </si>
+  <si>
+    <t>2012</t>
   </si>
 </sst>
 </file>
@@ -821,7 +827,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="253">
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
@@ -853,6 +859,24 @@
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
@@ -865,6 +889,12 @@
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
@@ -877,25 +907,854 @@
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -930,214 +1789,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
   </dxfs>
@@ -2316,17 +2967,88 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
           <a:ln>
             <a:noFill/>
           </a:ln>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2346,9 +3068,8 @@
               <a:pPr>
                 <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -2373,17 +3094,88 @@
       <c:pivotFmt>
         <c:idx val="1"/>
         <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
           <a:ln>
             <a:noFill/>
           </a:ln>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2403,9 +3195,8 @@
               <a:pPr>
                 <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -2430,17 +3221,88 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
+          <a:gradFill rotWithShape="1">
+            <a:gsLst>
+              <a:gs pos="0">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="103000"/>
+                  <a:lumMod val="102000"/>
+                  <a:tint val="94000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="50000">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="110000"/>
+                  <a:lumMod val="100000"/>
+                  <a:shade val="100000"/>
+                </a:schemeClr>
+              </a:gs>
+              <a:gs pos="100000">
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="99000"/>
+                  <a:satMod val="120000"/>
+                  <a:shade val="78000"/>
+                </a:schemeClr>
+              </a:gs>
+            </a:gsLst>
+            <a:lin ang="5400000" scaled="0"/>
+          </a:gradFill>
           <a:ln>
             <a:noFill/>
           </a:ln>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="none"/>
+          <c:symbol val="circle"/>
+          <c:size val="6"/>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2460,9 +3322,8 @@
               <a:pPr>
                 <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -2545,13 +3406,42 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
             <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -2686,13 +3576,42 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
             <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -2800,13 +3719,42 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
             <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -2935,9 +3883,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -2966,9 +3913,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2994,9 +3941,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -3036,9 +3982,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -3062,17 +4007,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -4239,51 +5195,58 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="294">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr/>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -4292,9 +5255,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4313,14 +5275,6 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -4329,20 +5283,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -4351,13 +5305,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4369,10 +5323,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="3">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -4381,16 +5335,17 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -4408,21 +5363,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4441,14 +5393,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -4460,14 +5411,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -4481,9 +5432,8 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4497,12 +5447,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -4514,9 +5458,9 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4531,14 +5475,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -4550,14 +5493,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -4569,14 +5512,13 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -4585,14 +5527,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -4600,7 +5541,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -4613,11 +5554,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr/>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -4625,14 +5566,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4644,12 +5585,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4665,7 +5613,6 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4674,9 +5621,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4692,14 +5638,13 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4708,9 +5653,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -4722,12 +5666,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -7421,8 +8359,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A24EFC77-32C8-42A7-823F-3DD147007D54}" name="Homework Pivot Table" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:E21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A24EFC77-32C8-42A7-823F-3DD147007D54}" name="Homework Pivot Table" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:E21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField showAll="0"/>
@@ -7514,9 +8452,9 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="111">
-        <item x="0"/>
-        <item x="3"/>
-        <item x="4"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
         <item x="6"/>
         <item x="7"/>
         <item x="8"/>
@@ -7607,27 +8545,27 @@
         <item x="94"/>
         <item x="95"/>
         <item x="87"/>
-        <item x="90"/>
-        <item x="97"/>
-        <item x="98"/>
-        <item x="91"/>
-        <item x="100"/>
-        <item x="93"/>
-        <item x="101"/>
-        <item x="96"/>
-        <item x="99"/>
-        <item x="104"/>
-        <item x="105"/>
-        <item x="106"/>
-        <item x="107"/>
-        <item x="108"/>
-        <item x="102"/>
-        <item x="109"/>
+        <item sd="0" x="90"/>
+        <item sd="0" x="97"/>
+        <item sd="0" x="98"/>
+        <item sd="0" x="91"/>
+        <item sd="0" x="100"/>
+        <item sd="0" x="93"/>
+        <item sd="0" x="101"/>
+        <item sd="0" x="96"/>
+        <item sd="0" x="99"/>
+        <item sd="0" x="104"/>
+        <item sd="0" x="105"/>
+        <item sd="0" x="106"/>
+        <item sd="0" x="107"/>
+        <item sd="0" x="108"/>
+        <item sd="0" x="102"/>
+        <item sd="0" x="109"/>
         <item x="103"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="15">
         <item x="0"/>
         <item sd="0" x="1"/>
@@ -7646,7 +8584,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item x="0"/>
         <item sd="0" x="1"/>
@@ -7657,7 +8595,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0">
+    <pivotField axis="axisPage" showAll="0">
       <items count="5">
         <item sd="0" x="0"/>
         <item sd="0" x="1"/>
@@ -7667,8 +8605,10 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="3">
     <field x="8"/>
+    <field x="9"/>
+    <field x="10"/>
   </rowFields>
   <rowItems count="17">
     <i>
@@ -7740,50 +8680,53 @@
       <x/>
     </i>
   </colItems>
+  <pageFields count="1">
+    <pageField fld="11" item="2" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="10">
-    <format dxfId="24">
+    <format dxfId="239">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="238">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="237">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="236">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="235">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="234">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="233">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="12">
+    <format dxfId="232">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="231">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="230">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
@@ -7830,17 +8773,6 @@
     </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleMedium20" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <filters count="1">
-    <filter fld="8" type="dateNewerThanOrEqual" evalOrder="-1" id="1">
-      <autoFilter ref="A1">
-        <filterColumn colId="0">
-          <customFilters>
-            <customFilter operator="greaterThanOrEqual" val="40909"/>
-          </customFilters>
-        </filterColumn>
-      </autoFilter>
-    </filter>
-  </filters>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -7853,18 +8785,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B346D0EA-AB1C-41C0-BBF0-2E96E1EFE38B}" name="EXPENSES" displayName="EXPENSES" ref="A2:I210" totalsRowShown="0" headerRowDxfId="25" dataDxfId="26" headerRowBorderDxfId="36" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B346D0EA-AB1C-41C0-BBF0-2E96E1EFE38B}" name="EXPENSES" displayName="EXPENSES" ref="A2:I210" totalsRowShown="0" headerRowDxfId="252" dataDxfId="250" headerRowBorderDxfId="251" tableBorderDxfId="249">
   <autoFilter ref="A2:I210" xr:uid="{B346D0EA-AB1C-41C0-BBF0-2E96E1EFE38B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D293012A-E6D3-46C2-BDDD-F9EDA417FB1A}" name="Document Date" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{C8DD84E8-96A3-4121-8FDD-4213D1497B3C}" name="Supplier" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{88D9CB0A-F694-4E3B-B894-B43948C3FF3A}" name="Reference" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{817BE148-4B32-44D8-923A-7EC94FFD115D}" name="Description" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{4B7E54C2-43C6-46C8-BFF1-26FCE2EEFF04}" name="Tax Inclusive Amount" dataDxfId="31" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{38C02688-9B32-40C1-8B82-0D0686F65BDE}" name="Column1" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{3AA8EA2C-B7F9-406D-941B-1D3B94FDFF85}" name="Bank Code" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{A1C6BEA9-1F4A-4858-B717-DC3C40BF8E51}" name="Account Code" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{DA88B93A-E597-4A57-A627-D80C8B8E93B9}" name="Payment Date" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{D293012A-E6D3-46C2-BDDD-F9EDA417FB1A}" name="Document Date" dataDxfId="248"/>
+    <tableColumn id="2" xr3:uid="{C8DD84E8-96A3-4121-8FDD-4213D1497B3C}" name="Supplier" dataDxfId="247"/>
+    <tableColumn id="3" xr3:uid="{88D9CB0A-F694-4E3B-B894-B43948C3FF3A}" name="Reference" dataDxfId="246"/>
+    <tableColumn id="4" xr3:uid="{817BE148-4B32-44D8-923A-7EC94FFD115D}" name="Description" dataDxfId="245"/>
+    <tableColumn id="5" xr3:uid="{4B7E54C2-43C6-46C8-BFF1-26FCE2EEFF04}" name="Tax Inclusive Amount" dataDxfId="244" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{38C02688-9B32-40C1-8B82-0D0686F65BDE}" name="Column1" dataDxfId="243"/>
+    <tableColumn id="7" xr3:uid="{3AA8EA2C-B7F9-406D-941B-1D3B94FDFF85}" name="Bank Code" dataDxfId="242"/>
+    <tableColumn id="8" xr3:uid="{A1C6BEA9-1F4A-4858-B717-DC3C40BF8E51}" name="Account Code" dataDxfId="241"/>
+    <tableColumn id="9" xr3:uid="{DA88B93A-E597-4A57-A627-D80C8B8E93B9}" name="Payment Date" dataDxfId="240"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14721,20 +15653,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A672D757-6117-4F49-978E-65FFB86648F5}">
-  <dimension ref="A3:E114"/>
+  <dimension ref="A1:E226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="31" customWidth="1"/>
-    <col min="3" max="4" width="16.7109375" style="30" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" t="s">
+        <v>171</v>
+      </c>
+    </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>168</v>
@@ -14742,6 +15683,7 @@
       <c r="B3" s="29" t="s">
         <v>169</v>
       </c>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
@@ -15005,284 +15947,254 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="30"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="30"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="30"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="30"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="30"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="30"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="30"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="30"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="30"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="30"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="30"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="30"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="30"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="30"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="30"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="30"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="30"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="30"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="30"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="30"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="30"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="30"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="30"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="30"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="30"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="30"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="30"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="30"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="30"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="30"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="30"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="30"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="30"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="30"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="30"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="30"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="30"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="30"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="30"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="30"/>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="30"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="30"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="30"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="30"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="30"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="30"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="30"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="30"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="30"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="30"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="30"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="30"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="30"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="30"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="30"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="30"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="30"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="30"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="30"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="30"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="30"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="30"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="30"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="30"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="30"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="30"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="30"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="30"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="30"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="30"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="30"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="30"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="30"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="30"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="30"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="30"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="30"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="30"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="30"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="30"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="30"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="30"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="30"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="30"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="30"/>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="30"/>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="30"/>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="30"/>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="30"/>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="30"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="30"/>
-    </row>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+    </row>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="154" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="158" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="159" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="161" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="164" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="165" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="166" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="167" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="168" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="169" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="170" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="171" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="172" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="173" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="174" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="175" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="176" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="177" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="178" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="179" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="180" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="181" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="182" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="183" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="184" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="185" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="186" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="187" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="188" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="189" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="190" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="191" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="192" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="193" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="194" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="195" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="196" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="197" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="198" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="199" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="200" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="201" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="202" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="203" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="204" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="205" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="206" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="207" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="208" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="209" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="210" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="211" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="212" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="213" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="214" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="215" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="216" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="217" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="218" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="219" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="220" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="221" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="222" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="223" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="224" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="225" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="226" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Updated Week 2 Homework charts
</commit_message>
<xml_diff>
--- a/AlexStrawn_Week2Homework.xlsx
+++ b/AlexStrawn_Week2Homework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theal\code\SavvyCoders\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{65FD5B77-8947-47C9-8705-3920350D2B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97A7BE02-831D-4FB8-BEC7-79F5976FB244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -565,7 +565,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,8 +634,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -669,8 +677,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -730,18 +744,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -773,21 +797,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -816,708 +839,23 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="8" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="1" xfId="8" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="7" borderId="1" xfId="8" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="20% - Accent5" xfId="7" builtinId="46"/>
-    <cellStyle name="Accent1" xfId="6" builtinId="29"/>
-    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
+  <cellStyles count="9">
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="40% - Accent4" xfId="8" builtinId="43"/>
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
-    <cellStyle name="Input" xfId="4" builtinId="20"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="7" builtinId="18"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="253">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
@@ -3006,49 +2344,7 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3133,49 +2429,7 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -3260,49 +2514,7 @@
           <a:sp3d/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -8359,7 +7571,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A24EFC77-32C8-42A7-823F-3DD147007D54}" name="Homework Pivot Table" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A24EFC77-32C8-42A7-823F-3DD147007D54}" name="Homework Pivot Table" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:E21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="14" showAll="0"/>
@@ -8687,46 +7899,46 @@
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="10">
-    <format dxfId="239">
+    <format dxfId="9">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="238">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="237">
+    <format dxfId="7">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="236">
+    <format dxfId="6">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="235">
+    <format dxfId="5">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="234">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="233">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0" selected="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="232">
+    <format dxfId="2">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="231">
+    <format dxfId="1">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="230">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
@@ -8785,18 +7997,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B346D0EA-AB1C-41C0-BBF0-2E96E1EFE38B}" name="EXPENSES" displayName="EXPENSES" ref="A2:I210" totalsRowShown="0" headerRowDxfId="252" dataDxfId="250" headerRowBorderDxfId="251" tableBorderDxfId="249">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B346D0EA-AB1C-41C0-BBF0-2E96E1EFE38B}" name="EXPENSES" displayName="EXPENSES" ref="A2:I210" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
   <autoFilter ref="A2:I210" xr:uid="{B346D0EA-AB1C-41C0-BBF0-2E96E1EFE38B}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D293012A-E6D3-46C2-BDDD-F9EDA417FB1A}" name="Document Date" dataDxfId="248"/>
-    <tableColumn id="2" xr3:uid="{C8DD84E8-96A3-4121-8FDD-4213D1497B3C}" name="Supplier" dataDxfId="247"/>
-    <tableColumn id="3" xr3:uid="{88D9CB0A-F694-4E3B-B894-B43948C3FF3A}" name="Reference" dataDxfId="246"/>
-    <tableColumn id="4" xr3:uid="{817BE148-4B32-44D8-923A-7EC94FFD115D}" name="Description" dataDxfId="245"/>
-    <tableColumn id="5" xr3:uid="{4B7E54C2-43C6-46C8-BFF1-26FCE2EEFF04}" name="Tax Inclusive Amount" dataDxfId="244" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{38C02688-9B32-40C1-8B82-0D0686F65BDE}" name="Column1" dataDxfId="243"/>
-    <tableColumn id="7" xr3:uid="{3AA8EA2C-B7F9-406D-941B-1D3B94FDFF85}" name="Bank Code" dataDxfId="242"/>
-    <tableColumn id="8" xr3:uid="{A1C6BEA9-1F4A-4858-B717-DC3C40BF8E51}" name="Account Code" dataDxfId="241"/>
-    <tableColumn id="9" xr3:uid="{DA88B93A-E597-4A57-A627-D80C8B8E93B9}" name="Payment Date" dataDxfId="240"/>
+    <tableColumn id="1" xr3:uid="{D293012A-E6D3-46C2-BDDD-F9EDA417FB1A}" name="Document Date" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{C8DD84E8-96A3-4121-8FDD-4213D1497B3C}" name="Supplier" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{88D9CB0A-F694-4E3B-B894-B43948C3FF3A}" name="Reference" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{817BE148-4B32-44D8-923A-7EC94FFD115D}" name="Description" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{4B7E54C2-43C6-46C8-BFF1-26FCE2EEFF04}" name="Tax Inclusive Amount" dataDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{38C02688-9B32-40C1-8B82-0D0686F65BDE}" name="Column1" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{3AA8EA2C-B7F9-406D-941B-1D3B94FDFF85}" name="Bank Code" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{A1C6BEA9-1F4A-4858-B717-DC3C40BF8E51}" name="Account Code" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{DA88B93A-E597-4A57-A627-D80C8B8E93B9}" name="Payment Date" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9127,31 +8339,31 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" s="10" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="24" t="s">
         <v>8</v>
       </c>
     </row>
@@ -15205,260 +14417,260 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="18">
         <v>12</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="18">
         <v>85</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>11</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="18">
         <v>72</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="18">
         <v>13</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="18">
         <v>60</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="18">
         <v>12</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="18">
         <v>95</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="18">
         <v>14</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="18">
         <v>88</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="18">
         <v>12</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <v>99</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="18">
         <v>11</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="18">
         <v>75</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="18">
         <v>13</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>100</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="18">
         <v>13</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>75</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="18">
         <v>15</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <v>85</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="18">
         <v>11</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="18">
         <v>85</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="16">
+      <c r="B16" s="16"/>
+      <c r="C16" s="15">
         <f>MIN(C4:C14)</f>
         <v>11</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="15">
         <f>MIN(D4:D14)</f>
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="16">
+      <c r="B17" s="16"/>
+      <c r="C17" s="15">
         <f>MAX(C4:C14)</f>
         <v>15</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="15">
         <f>MAX(D4:D14)</f>
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="16">
+      <c r="B18" s="16"/>
+      <c r="C18" s="15">
         <f>AVERAGE(C4:C14)</f>
         <v>12.454545454545455</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D18" s="15">
         <f>AVERAGE(D4:D14)</f>
         <v>83.545454545454547</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="16">
+      <c r="B19" s="16"/>
+      <c r="C19" s="15">
         <f>MODE(C4:C14)</f>
         <v>12</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D19" s="15">
         <f>MODE(D4:D14)</f>
         <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="16">
+      <c r="B20" s="16"/>
+      <c r="C20" s="15">
         <f>MEDIAN(C4:C14)</f>
         <v>12</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="15">
         <f>MEDIAN(D4:D14)</f>
         <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="B21" s="17"/>
-      <c r="C21" s="16">
+      <c r="B21" s="16"/>
+      <c r="C21" s="15">
         <f>COUNT(C4:C14)</f>
         <v>11</v>
       </c>
-      <c r="D21" s="16">
+      <c r="D21" s="15">
         <f>COUNT(D4:D14)</f>
         <v>11</v>
       </c>
@@ -15472,8 +14684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C856F3-1A38-4E44-95E4-277990A43875}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15493,154 +14705,154 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="31" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="33">
         <v>2000</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="34">
         <v>0.21</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="32">
         <v>3</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="33">
         <f>B4*C4</f>
         <v>420</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="33">
         <f>E4+B4</f>
         <v>2420</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="33">
         <f>F4/D4</f>
         <v>806.66666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="33">
         <v>450</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="34">
         <v>0.25</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="32">
         <v>3</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="33">
         <f>B5*C5</f>
         <v>112.5</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="33">
         <f>E5+B5</f>
         <v>562.5</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="33">
         <f>F5/D5</f>
         <v>187.5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="33">
         <v>975</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="34">
         <v>0.27</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="32">
         <v>3</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="33">
         <f>B6*C6</f>
         <v>263.25</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="33">
         <f>E6+B6</f>
         <v>1238.25</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="33">
         <f>F6/D6</f>
         <v>412.75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="33">
         <v>1500</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="34">
         <v>0.15</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="32">
         <v>3</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="33">
         <f>B7*C7</f>
         <v>225</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="33">
         <f>E7+B7</f>
         <v>1725</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="33">
         <f>F7/D7</f>
         <v>575</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="33">
         <v>780</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="34">
         <v>0.25</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="32">
         <v>3</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="33">
         <f>B8*C8</f>
         <v>195</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="33">
         <f>E8+B8</f>
         <v>975</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="33">
         <f>F8/D8</f>
         <v>325</v>
       </c>
@@ -15655,21 +14867,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A672D757-6117-4F49-978E-65FFB86648F5}">
   <dimension ref="A1:E226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="29" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>170</v>
       </c>
       <c r="B1" t="s">
@@ -15677,25 +14889,25 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="28" t="s">
         <v>169</v>
       </c>
-      <c r="E3" s="30"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="29" t="s">
         <v>39</v>
       </c>
       <c r="E4" t="s">
@@ -15703,55 +14915,55 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+      <c r="A5" s="26">
         <v>40910</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="30">
         <v>1000</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
       <c r="E5" s="14">
         <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="27">
+      <c r="A6" s="26">
         <v>40913</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="30">
         <v>340</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
       <c r="E6" s="14">
         <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="27">
+      <c r="A7" s="26">
         <v>40923</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="30">
         <v>80</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="30">
         <v>35</v>
       </c>
-      <c r="D7" s="31"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="14">
         <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
+      <c r="A8" s="26">
         <v>40924</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="30">
         <v>1392</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31">
+      <c r="C8" s="30"/>
+      <c r="D8" s="30">
         <v>105</v>
       </c>
       <c r="E8" s="14">
@@ -15759,26 +14971,26 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="27">
+      <c r="A9" s="26">
         <v>40928</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="30">
         <v>20000</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="30">
         <v>-20000</v>
       </c>
-      <c r="D9" s="31"/>
+      <c r="D9" s="30"/>
       <c r="E9" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
+      <c r="A10" s="26">
         <v>40929</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31">
+      <c r="C10" s="30"/>
+      <c r="D10" s="30">
         <v>61</v>
       </c>
       <c r="E10" s="14">
@@ -15786,29 +14998,29 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
+      <c r="A11" s="26">
         <v>40934</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="30">
         <v>6720</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="30">
         <v>20000</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="30"/>
       <c r="E11" s="14">
         <v>26720</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
+      <c r="A12" s="26">
         <v>40939</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="30">
         <v>738.25</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31">
+      <c r="C12" s="30"/>
+      <c r="D12" s="30">
         <v>-170</v>
       </c>
       <c r="E12" s="14">
@@ -15816,70 +15028,70 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
+      <c r="A13" s="26">
         <v>40941</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="30">
         <v>1000</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
       <c r="E13" s="14">
         <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
+      <c r="A14" s="26">
         <v>40944</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="30">
         <v>340</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="14">
         <v>340</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
+      <c r="A15" s="26">
         <v>40954</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="30">
         <v>80</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="30">
         <v>35</v>
       </c>
-      <c r="D15" s="31"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="14">
         <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
+      <c r="A16" s="26">
         <v>40959</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="30">
         <v>20000</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="30">
         <v>-20000</v>
       </c>
-      <c r="D16" s="31"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="14">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="27">
+      <c r="A17" s="26">
         <v>40964</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="30">
         <v>2200</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30">
         <v>75</v>
       </c>
       <c r="E17" s="14">
@@ -15887,42 +15099,42 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="27">
+      <c r="A18" s="26">
         <v>40965</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="30">
         <v>6720</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="30">
         <v>20000</v>
       </c>
-      <c r="D18" s="31"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="14">
         <v>26720</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="27">
+      <c r="A19" s="26">
         <v>40966</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B19" s="30">
         <v>514</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="14">
         <v>514</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="27">
+      <c r="A20" s="26">
         <v>40968</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="30">
         <v>3770</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31">
+      <c r="C20" s="30"/>
+      <c r="D20" s="30">
         <v>-70</v>
       </c>
       <c r="E20" s="14">
@@ -15930,16 +15142,16 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="27" t="s">
         <v>167</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="30">
         <v>64894.25</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="30">
         <v>70</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="30">
         <v>1</v>
       </c>
       <c r="E21" s="14">

</xml_diff>

<commit_message>
Updated Week 2 Homework to reflect correct Spreadsheet
</commit_message>
<xml_diff>
--- a/AlexStrawn_Week2Homework.xlsx
+++ b/AlexStrawn_Week2Homework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theal\code\SavvyCoders\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97A7BE02-831D-4FB8-BEC7-79F5976FB244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D774BB4-7963-44E9-A032-80B58E7CE849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14685,7 +14685,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>